<commit_message>
~ changes in configuration files
</commit_message>
<xml_diff>
--- a/examples/oucru/oucru-13dx/resources/outputs/templates/ccfgs_13dx_data_fixed.xlsx
+++ b/examples/oucru/oucru-13dx/resources/outputs/templates/ccfgs_13dx_data_fixed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cbit/Desktop/repositories/github/datablend/main/examples/oucru/oucru-13dx/resources/outputs/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F4D0DC-A000-9F46-A9D7-F42F51B39E57}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B907A6-6FED-9447-8A78-45E88D61E9CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35840" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="460" windowWidth="35060" windowHeight="21940" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ENROL" sheetId="1" r:id="rId1"/>
@@ -2542,9 +2542,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="117.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -3438,7 +3454,7 @@
   <dimension ref="A1:L94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5078,9 +5094,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -5259,9 +5291,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -5480,9 +5527,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -6142,9 +6205,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
~ improving ccfgs and cleaning DR, DF, MD
</commit_message>
<xml_diff>
--- a/examples/oucru/oucru-13dx/resources/outputs/templates/ccfgs_13dx_data_fixed.xlsx
+++ b/examples/oucru/oucru-13dx/resources/outputs/templates/ccfgs_13dx_data_fixed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cbit/Desktop/repositories/github/datablend/main/examples/oucru/oucru-13dx/resources/outputs/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kelda\Desktop\repositories\github\datablend\main\examples\oucru\oucru-13dx\resources\outputs\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B907A6-6FED-9447-8A78-45E88D61E9CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{797A471D-4D2D-4CBD-992B-57CE6C968CC9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="460" windowWidth="35060" windowHeight="21940" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ENROL" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1087" uniqueCount="452">
   <si>
     <t>from_name</t>
   </si>
@@ -466,9 +466,6 @@
     <t>lethargy</t>
   </si>
   <si>
-    <t>breath</t>
-  </si>
-  <si>
     <t>skin_clammy</t>
   </si>
   <si>
@@ -1036,9 +1033,6 @@
     <t>event_shock</t>
   </si>
   <si>
-    <t>event_death</t>
-  </si>
-  <si>
     <t>SampleNo</t>
   </si>
   <si>
@@ -1358,6 +1352,39 @@
   </si>
   <si>
     <t>event_pcr</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>or admission?? Compare</t>
+  </si>
+  <si>
+    <t>skin_Rash?</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>shortness_of_breath</t>
+  </si>
+  <si>
+    <t>ignore cumulative of previous</t>
+  </si>
+  <si>
+    <t>careful is boolean!</t>
+  </si>
+  <si>
+    <t>units?</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>date discharge when death? Or date discharge or date_death?</t>
+  </si>
+  <si>
+    <t>event_discharge</t>
   </si>
 </sst>
 </file>
@@ -1381,15 +1408,33 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1412,15 +1457,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1759,17 +1821,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M43"/>
+  <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="2" width="25.83203125" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1809,8 +1884,11 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N1" s="2" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1827,7 +1905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1841,7 +1919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1855,7 +1933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1869,7 +1947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1886,7 +1964,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1903,7 +1981,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1920,7 +1998,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1934,7 +2012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1948,7 +2026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1962,7 +2040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -1982,7 +2060,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1996,7 +2074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -2016,7 +2094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -2030,7 +2108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -2044,7 +2122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -2058,7 +2136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -2075,7 +2153,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -2092,7 +2170,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -2112,7 +2190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -2132,7 +2210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -2152,7 +2230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -2172,7 +2250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -2192,7 +2270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -2212,7 +2290,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>37</v>
       </c>
@@ -2232,7 +2310,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>38</v>
       </c>
@@ -2252,7 +2330,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -2269,7 +2347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -2289,7 +2367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>41</v>
       </c>
@@ -2306,7 +2384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>42</v>
       </c>
@@ -2323,7 +2401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>43</v>
       </c>
@@ -2340,7 +2418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>44</v>
       </c>
@@ -2357,7 +2435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>45</v>
       </c>
@@ -2374,7 +2452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>46</v>
       </c>
@@ -2391,7 +2469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>47</v>
       </c>
@@ -2405,7 +2483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>48</v>
       </c>
@@ -2419,7 +2497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>49</v>
       </c>
@@ -2439,7 +2517,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>50</v>
       </c>
@@ -2453,7 +2531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>51</v>
       </c>
@@ -2470,7 +2548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>52</v>
       </c>
@@ -2487,7 +2565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>53</v>
       </c>
@@ -2510,27 +2588,30 @@
         <v>110</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+    <row r="43" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="F43" t="b">
+      <c r="F43" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="G43" t="s">
+      <c r="G43" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H43" t="s">
+      <c r="H43" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="K43" t="s">
+      <c r="K43" s="3" t="s">
         <v>111</v>
+      </c>
+      <c r="N43" s="3" t="s">
+        <v>442</v>
       </c>
     </row>
   </sheetData>
@@ -2542,27 +2623,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="117.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="117.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2600,7 +2681,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -2614,12 +2695,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B3" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C3" t="s">
         <v>94</v>
@@ -2628,12 +2709,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B4" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C4" t="s">
         <v>96</v>
@@ -2642,214 +2723,214 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="F5" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>421</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="F6" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>408</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B7" s="3" t="s">
         <v>422</v>
       </c>
-      <c r="C5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="C7" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>433</v>
       </c>
-      <c r="F5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="F7" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B8" s="3" t="s">
         <v>423</v>
       </c>
-      <c r="C6" t="s">
-        <v>92</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="C8" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>434</v>
       </c>
-      <c r="F6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="F8" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>410</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B9" s="3" t="s">
         <v>424</v>
       </c>
-      <c r="C7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="C9" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F9" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>425</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>435</v>
       </c>
-      <c r="F7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>411</v>
-      </c>
-      <c r="B8" t="s">
-        <v>425</v>
-      </c>
-      <c r="C8" t="s">
-        <v>92</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="F10" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>426</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="F11" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>427</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F12" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>436</v>
       </c>
-      <c r="F8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>412</v>
-      </c>
-      <c r="B9" t="s">
-        <v>426</v>
-      </c>
-      <c r="C9" t="s">
-        <v>96</v>
-      </c>
-      <c r="F9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>413</v>
-      </c>
-      <c r="B10" t="s">
-        <v>427</v>
-      </c>
-      <c r="C10" t="s">
-        <v>92</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="F13" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>437</v>
       </c>
-      <c r="F10" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>414</v>
-      </c>
-      <c r="B11" t="s">
-        <v>428</v>
-      </c>
-      <c r="C11" t="s">
-        <v>92</v>
-      </c>
-      <c r="D11" t="s">
-        <v>437</v>
-      </c>
-      <c r="F11" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>415</v>
-      </c>
-      <c r="B12" t="s">
-        <v>429</v>
-      </c>
-      <c r="C12" t="s">
-        <v>96</v>
-      </c>
-      <c r="F12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="F14" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>416</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B15" t="s">
         <v>430</v>
-      </c>
-      <c r="C13" t="s">
-        <v>92</v>
-      </c>
-      <c r="D13" t="s">
-        <v>438</v>
-      </c>
-      <c r="F13" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>417</v>
-      </c>
-      <c r="B14" t="s">
-        <v>431</v>
-      </c>
-      <c r="C14" t="s">
-        <v>92</v>
-      </c>
-      <c r="D14" t="s">
-        <v>439</v>
-      </c>
-      <c r="F14" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>418</v>
-      </c>
-      <c r="B15" t="s">
-        <v>432</v>
       </c>
       <c r="C15" t="s">
         <v>93</v>
       </c>
       <c r="D15" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E15" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="F15" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>417</v>
+      </c>
+      <c r="B16" t="s">
+        <v>417</v>
+      </c>
+      <c r="C16" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" t="s">
+        <v>439</v>
+      </c>
+      <c r="E16" t="s">
         <v>419</v>
       </c>
-      <c r="B16" t="s">
-        <v>419</v>
-      </c>
-      <c r="C16" t="s">
-        <v>92</v>
-      </c>
-      <c r="D16" t="s">
-        <v>441</v>
-      </c>
-      <c r="E16" t="s">
-        <v>421</v>
-      </c>
       <c r="F16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>52</v>
       </c>
@@ -2873,30 +2954,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M31"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="A22" sqref="A22:XFD23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2936,8 +3017,11 @@
       <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N1" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -2951,7 +3035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>112</v>
       </c>
@@ -2962,13 +3046,13 @@
         <v>92</v>
       </c>
       <c r="D3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>113</v>
       </c>
@@ -2982,24 +3066,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D5" t="s">
-        <v>150</v>
-      </c>
-      <c r="F5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C5" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="F5" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>115</v>
       </c>
@@ -3010,13 +3094,13 @@
         <v>92</v>
       </c>
       <c r="D6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F6" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>116</v>
       </c>
@@ -3030,7 +3114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>117</v>
       </c>
@@ -3044,7 +3128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>118</v>
       </c>
@@ -3064,7 +3148,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -3084,7 +3168,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>119</v>
       </c>
@@ -3095,13 +3179,13 @@
         <v>92</v>
       </c>
       <c r="D11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F11" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>120</v>
       </c>
@@ -3118,7 +3202,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -3135,7 +3219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -3152,7 +3236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>121</v>
       </c>
@@ -3169,7 +3253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>122</v>
       </c>
@@ -3186,7 +3270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>123</v>
       </c>
@@ -3203,12 +3287,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>124</v>
       </c>
       <c r="B18" t="s">
-        <v>145</v>
+        <v>445</v>
       </c>
       <c r="C18" t="s">
         <v>95</v>
@@ -3220,43 +3304,49 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="19" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="F19" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="N19" s="5" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="E19" t="s">
-        <v>132</v>
-      </c>
-      <c r="F19" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>126</v>
-      </c>
-      <c r="B20" t="s">
-        <v>147</v>
-      </c>
-      <c r="C20" t="s">
-        <v>95</v>
-      </c>
-      <c r="F20" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F20" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="N20" s="3" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>127</v>
       </c>
       <c r="B21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C21" t="s">
         <v>95</v>
@@ -3265,7 +3355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>128</v>
       </c>
@@ -3282,7 +3372,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>129</v>
       </c>
@@ -3299,7 +3389,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>130</v>
       </c>
@@ -3313,7 +3403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>131</v>
       </c>
@@ -3333,7 +3423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>52</v>
       </c>
@@ -3350,7 +3440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>17</v>
       </c>
@@ -3367,7 +3457,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>18</v>
       </c>
@@ -3384,7 +3474,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>53</v>
       </c>
@@ -3404,7 +3494,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>132</v>
       </c>
@@ -3424,7 +3514,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>133</v>
       </c>
@@ -3451,28 +3541,28 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:L94"/>
+  <dimension ref="A1:M94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="E90" sqref="E90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="79.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="79.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3510,7 +3600,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -3524,7 +3614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -3538,12 +3628,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C4" t="s">
         <v>96</v>
@@ -3552,9 +3642,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B5" t="s">
         <v>61</v>
@@ -3566,12 +3656,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C6" t="s">
         <v>93</v>
@@ -3580,12 +3670,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C7" t="s">
         <v>93</v>
@@ -3594,12 +3684,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C8" t="s">
         <v>93</v>
@@ -3608,7 +3698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -3619,7 +3709,7 @@
         <v>93</v>
       </c>
       <c r="E9" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F9" t="b">
         <v>0</v>
@@ -3628,7 +3718,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -3642,7 +3732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -3653,16 +3743,16 @@
         <v>92</v>
       </c>
       <c r="D11" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F11" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>118</v>
       </c>
@@ -3679,12 +3769,12 @@
         <v>109</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B13" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C13" t="s">
         <v>93</v>
@@ -3693,32 +3783,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>158</v>
+      </c>
+      <c r="B14" t="s">
+        <v>242</v>
+      </c>
+      <c r="C14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D14" t="s">
+        <v>319</v>
+      </c>
+      <c r="E14" t="s">
+        <v>237</v>
+      </c>
+      <c r="F14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>159</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>243</v>
-      </c>
-      <c r="C14" t="s">
-        <v>92</v>
-      </c>
-      <c r="D14" t="s">
-        <v>320</v>
-      </c>
-      <c r="E14" t="s">
-        <v>238</v>
-      </c>
-      <c r="F14" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>160</v>
-      </c>
-      <c r="B15" t="s">
-        <v>244</v>
       </c>
       <c r="C15" t="s">
         <v>92</v>
@@ -3727,18 +3817,18 @@
         <v>100</v>
       </c>
       <c r="E15" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F15" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B16" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C16" t="s">
         <v>96</v>
@@ -3747,55 +3837,55 @@
         <v>1</v>
       </c>
       <c r="L16" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B17" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C17" t="s">
         <v>93</v>
       </c>
       <c r="E17" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F17" t="b">
         <v>0</v>
       </c>
       <c r="K17" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B18" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C18" t="s">
         <v>93</v>
       </c>
       <c r="E18" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F18" t="b">
         <v>0</v>
       </c>
       <c r="K18" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B19" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C19" t="s">
         <v>92</v>
@@ -3804,58 +3894,58 @@
         <v>100</v>
       </c>
       <c r="E19" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F19" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B20" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C20" t="s">
         <v>93</v>
       </c>
       <c r="E20" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F20" t="b">
         <v>0</v>
       </c>
       <c r="K20" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>165</v>
+      </c>
+      <c r="B21" t="s">
+        <v>249</v>
+      </c>
+      <c r="C21" t="s">
+        <v>92</v>
+      </c>
+      <c r="D21" t="s">
+        <v>320</v>
+      </c>
+      <c r="E21" t="s">
+        <v>237</v>
+      </c>
+      <c r="F21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>166</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>250</v>
-      </c>
-      <c r="C21" t="s">
-        <v>92</v>
-      </c>
-      <c r="D21" t="s">
-        <v>321</v>
-      </c>
-      <c r="E21" t="s">
-        <v>238</v>
-      </c>
-      <c r="F21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>167</v>
-      </c>
-      <c r="B22" t="s">
-        <v>251</v>
       </c>
       <c r="C22" t="s">
         <v>92</v>
@@ -3864,38 +3954,38 @@
         <v>100</v>
       </c>
       <c r="E22" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F22" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>167</v>
+      </c>
+      <c r="B23" t="s">
+        <v>251</v>
+      </c>
+      <c r="C23" t="s">
+        <v>92</v>
+      </c>
+      <c r="D23" t="s">
+        <v>321</v>
+      </c>
+      <c r="E23" t="s">
+        <v>252</v>
+      </c>
+      <c r="F23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>168</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>252</v>
-      </c>
-      <c r="C23" t="s">
-        <v>92</v>
-      </c>
-      <c r="D23" t="s">
-        <v>322</v>
-      </c>
-      <c r="E23" t="s">
-        <v>253</v>
-      </c>
-      <c r="F23" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>169</v>
-      </c>
-      <c r="B24" t="s">
-        <v>253</v>
       </c>
       <c r="C24" t="s">
         <v>96</v>
@@ -3904,9 +3994,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B25" t="s">
         <v>77</v>
@@ -3915,304 +4005,313 @@
         <v>95</v>
       </c>
       <c r="E25" t="s">
+        <v>252</v>
+      </c>
+      <c r="F25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>170</v>
+      </c>
+      <c r="B26" t="s">
         <v>253</v>
-      </c>
-      <c r="F25" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>171</v>
-      </c>
-      <c r="B26" t="s">
-        <v>254</v>
       </c>
       <c r="C26" t="s">
         <v>95</v>
       </c>
       <c r="E26" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F26" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B27" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C27" t="s">
         <v>95</v>
       </c>
       <c r="E27" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F27" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B28" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C28" t="s">
         <v>95</v>
       </c>
       <c r="E28" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F28" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B29" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C29" t="s">
         <v>95</v>
       </c>
       <c r="E29" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F29" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B30" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C30" t="s">
         <v>95</v>
       </c>
       <c r="E30" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F30" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B31" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C31" t="s">
         <v>95</v>
       </c>
       <c r="E31" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F31" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>176</v>
+      </c>
+      <c r="B32" t="s">
+        <v>259</v>
+      </c>
+      <c r="C32" t="s">
+        <v>92</v>
+      </c>
+      <c r="D32" t="s">
+        <v>322</v>
+      </c>
+      <c r="F32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="C32" t="s">
-        <v>92</v>
-      </c>
-      <c r="D32" t="s">
-        <v>323</v>
-      </c>
-      <c r="F32" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="C33" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="F33" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="C33" t="s">
-        <v>92</v>
-      </c>
-      <c r="D33" t="s">
-        <v>100</v>
-      </c>
-      <c r="F33" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+      <c r="C34" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F34" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C35" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="F34" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+      <c r="E35" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="F35" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="M35" s="5" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="E35" t="s">
-        <v>238</v>
-      </c>
-      <c r="F35" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+      <c r="E36" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="F36" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="M36" s="5" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="E36" t="s">
-        <v>238</v>
-      </c>
-      <c r="F36" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+      <c r="E37" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="F37" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="M37" s="5" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>182</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>265</v>
-      </c>
-      <c r="C37" t="s">
-        <v>95</v>
-      </c>
-      <c r="E37" t="s">
-        <v>238</v>
-      </c>
-      <c r="F37" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>183</v>
-      </c>
-      <c r="B38" t="s">
-        <v>266</v>
       </c>
       <c r="C38" t="s">
         <v>95</v>
       </c>
       <c r="E38" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F38" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B39" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C39" t="s">
         <v>95</v>
       </c>
       <c r="E39" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F39" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B40" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C40" t="s">
         <v>95</v>
       </c>
       <c r="E40" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F40" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B41" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C41" t="s">
         <v>95</v>
       </c>
       <c r="E41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F41" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B42" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C42" t="s">
         <v>95</v>
       </c>
       <c r="E42" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F42" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B43" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C43" t="s">
         <v>94</v>
@@ -4221,12 +4320,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B44" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C44" t="s">
         <v>92</v>
@@ -4235,18 +4334,18 @@
         <v>101</v>
       </c>
       <c r="E44" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F44" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B45" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C45" t="s">
         <v>96</v>
@@ -4255,12 +4354,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B46" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C46" t="s">
         <v>92</v>
@@ -4269,18 +4368,18 @@
         <v>100</v>
       </c>
       <c r="E46" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F46" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B47" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C47" t="s">
         <v>92</v>
@@ -4289,78 +4388,78 @@
         <v>101</v>
       </c>
       <c r="E47" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F47" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>192</v>
+      </c>
+      <c r="B48" t="s">
+        <v>275</v>
+      </c>
+      <c r="C48" t="s">
+        <v>92</v>
+      </c>
+      <c r="D48" t="s">
+        <v>323</v>
+      </c>
+      <c r="E48" t="s">
+        <v>272</v>
+      </c>
+      <c r="F48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>193</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>276</v>
       </c>
-      <c r="C48" t="s">
-        <v>92</v>
-      </c>
-      <c r="D48" t="s">
+      <c r="C49" t="s">
+        <v>92</v>
+      </c>
+      <c r="D49" t="s">
         <v>324</v>
       </c>
-      <c r="E48" t="s">
-        <v>273</v>
-      </c>
-      <c r="F48" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+      <c r="E49" t="s">
+        <v>272</v>
+      </c>
+      <c r="F49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>194</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>277</v>
       </c>
-      <c r="C49" t="s">
-        <v>92</v>
-      </c>
-      <c r="D49" t="s">
+      <c r="C50" t="s">
+        <v>92</v>
+      </c>
+      <c r="D50" t="s">
         <v>325</v>
       </c>
-      <c r="E49" t="s">
-        <v>273</v>
-      </c>
-      <c r="F49" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+      <c r="E50" t="s">
+        <v>272</v>
+      </c>
+      <c r="F50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>195</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B51" t="s">
         <v>278</v>
-      </c>
-      <c r="C50" t="s">
-        <v>92</v>
-      </c>
-      <c r="D50" t="s">
-        <v>326</v>
-      </c>
-      <c r="E50" t="s">
-        <v>273</v>
-      </c>
-      <c r="F50" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>196</v>
-      </c>
-      <c r="B51" t="s">
-        <v>279</v>
       </c>
       <c r="C51" t="s">
         <v>95</v>
@@ -4369,12 +4468,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B52" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C52" t="s">
         <v>92</v>
@@ -4383,38 +4482,41 @@
         <v>100</v>
       </c>
       <c r="E52" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F52" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+    <row r="53" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="F53" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="M53" s="5" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>198</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B54" t="s">
         <v>281</v>
-      </c>
-      <c r="C53" t="s">
-        <v>92</v>
-      </c>
-      <c r="D53" t="s">
-        <v>101</v>
-      </c>
-      <c r="E53" t="s">
-        <v>282</v>
-      </c>
-      <c r="F53" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>199</v>
-      </c>
-      <c r="B54" t="s">
-        <v>282</v>
       </c>
       <c r="C54" t="s">
         <v>96</v>
@@ -4423,12 +4525,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B55" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C55" t="s">
         <v>92</v>
@@ -4437,18 +4539,18 @@
         <v>100</v>
       </c>
       <c r="E55" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F55" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B56" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C56" t="s">
         <v>92</v>
@@ -4457,18 +4559,18 @@
         <v>100</v>
       </c>
       <c r="E56" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F56" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B57" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C57" t="s">
         <v>92</v>
@@ -4477,18 +4579,18 @@
         <v>101</v>
       </c>
       <c r="E57" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F57" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B58" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C58" t="s">
         <v>96</v>
@@ -4497,63 +4599,63 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B59" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C59" t="s">
         <v>95</v>
       </c>
       <c r="E59" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F59" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B60" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C60" t="s">
         <v>95</v>
       </c>
       <c r="E60" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F60" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B61" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C61" t="s">
         <v>95</v>
       </c>
       <c r="E61" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F61" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B62" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C62" t="s">
         <v>95</v>
@@ -4562,29 +4664,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>207</v>
+      </c>
+      <c r="B63" t="s">
+        <v>290</v>
+      </c>
+      <c r="C63" t="s">
+        <v>92</v>
+      </c>
+      <c r="D63" t="s">
+        <v>326</v>
+      </c>
+      <c r="F63" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>208</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B64" t="s">
         <v>291</v>
-      </c>
-      <c r="C63" t="s">
-        <v>92</v>
-      </c>
-      <c r="D63" t="s">
-        <v>327</v>
-      </c>
-      <c r="F63" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>209</v>
-      </c>
-      <c r="B64" t="s">
-        <v>292</v>
       </c>
       <c r="C64" t="s">
         <v>92</v>
@@ -4593,18 +4695,18 @@
         <v>101</v>
       </c>
       <c r="E64" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F64" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B65" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C65" t="s">
         <v>96</v>
@@ -4613,29 +4715,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>210</v>
+      </c>
+      <c r="B66" t="s">
+        <v>293</v>
+      </c>
+      <c r="C66" t="s">
+        <v>92</v>
+      </c>
+      <c r="D66" t="s">
+        <v>327</v>
+      </c>
+      <c r="F66" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>211</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B67" t="s">
         <v>294</v>
-      </c>
-      <c r="C66" t="s">
-        <v>92</v>
-      </c>
-      <c r="D66" t="s">
-        <v>328</v>
-      </c>
-      <c r="F66" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>212</v>
-      </c>
-      <c r="B67" t="s">
-        <v>295</v>
       </c>
       <c r="C67" t="s">
         <v>92</v>
@@ -4644,30 +4746,30 @@
         <v>101</v>
       </c>
       <c r="E67" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F67" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B68" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C68" t="s">
         <v>95</v>
       </c>
       <c r="E68" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F68" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>31</v>
       </c>
@@ -4678,52 +4780,52 @@
         <v>95</v>
       </c>
       <c r="E69" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F69" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B70" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C70" t="s">
         <v>95</v>
       </c>
       <c r="E70" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F70" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B71" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C71" t="s">
         <v>95</v>
       </c>
       <c r="E71" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F71" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B72" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C72" t="s">
         <v>95</v>
@@ -4732,12 +4834,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B73" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C73" t="s">
         <v>94</v>
@@ -4746,147 +4848,147 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
+    <row r="74" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F74" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B75" s="4" t="s">
         <v>301</v>
       </c>
-      <c r="C74" t="s">
-        <v>96</v>
-      </c>
-      <c r="F74" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
+      <c r="C75" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F75" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B76" s="4" t="s">
         <v>302</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C76" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="F75" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
+      <c r="F76" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B77" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C77" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="F76" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
+      <c r="F77" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B78" s="4" t="s">
         <v>304</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C78" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="F77" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
+      <c r="F78" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B79" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C79" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F79" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="C80" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="F78" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
-        <v>223</v>
-      </c>
-      <c r="B79" t="s">
-        <v>306</v>
-      </c>
-      <c r="C79" t="s">
-        <v>92</v>
-      </c>
-      <c r="F79" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
+      <c r="F80" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B81" s="4" t="s">
         <v>307</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C81" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="F80" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
+      <c r="E81" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="F81" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>225</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B82" t="s">
         <v>308</v>
-      </c>
-      <c r="C81" t="s">
-        <v>93</v>
-      </c>
-      <c r="E81" t="s">
-        <v>238</v>
-      </c>
-      <c r="F81" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
-        <v>226</v>
-      </c>
-      <c r="B82" t="s">
-        <v>309</v>
       </c>
       <c r="C82" t="s">
         <v>93</v>
       </c>
       <c r="E82" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F82" t="b">
         <v>0</v>
       </c>
       <c r="K82" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B83" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C83" t="s">
         <v>93</v>
@@ -4895,49 +4997,49 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B84" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C84" t="s">
         <v>93</v>
       </c>
       <c r="E84" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F84" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B85" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C85" t="s">
         <v>93</v>
       </c>
       <c r="E85" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F85" t="b">
         <v>0</v>
       </c>
       <c r="K85" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B86" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C86" t="s">
         <v>93</v>
@@ -4946,32 +5048,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
+        <v>230</v>
+      </c>
+      <c r="B87" t="s">
+        <v>313</v>
+      </c>
+      <c r="C87" t="s">
+        <v>92</v>
+      </c>
+      <c r="D87" t="s">
+        <v>328</v>
+      </c>
+      <c r="E87" t="s">
+        <v>315</v>
+      </c>
+      <c r="F87" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>231</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B88" t="s">
         <v>314</v>
-      </c>
-      <c r="C87" t="s">
-        <v>92</v>
-      </c>
-      <c r="D87" t="s">
-        <v>329</v>
-      </c>
-      <c r="E87" t="s">
-        <v>316</v>
-      </c>
-      <c r="F87" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
-        <v>232</v>
-      </c>
-      <c r="B88" t="s">
-        <v>315</v>
       </c>
       <c r="C88" t="s">
         <v>94</v>
@@ -4980,46 +5082,49 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
+    <row r="89" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="B89" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="C89" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F89" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L89" s="5" t="s">
+        <v>451</v>
+      </c>
+      <c r="M89" s="5" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>233</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B90" t="s">
         <v>316</v>
-      </c>
-      <c r="C89" t="s">
-        <v>96</v>
-      </c>
-      <c r="F89" t="b">
-        <v>1</v>
-      </c>
-      <c r="L89" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
-        <v>234</v>
-      </c>
-      <c r="B90" t="s">
-        <v>317</v>
       </c>
       <c r="C90" t="s">
         <v>94</v>
       </c>
       <c r="E90" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F90" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B91" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C91" t="s">
         <v>96</v>
@@ -5028,7 +5133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>52</v>
       </c>
@@ -5045,12 +5150,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B93" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C93" t="s">
         <v>96</v>
@@ -5059,18 +5164,18 @@
         <v>1</v>
       </c>
       <c r="I93" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="J93" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B94" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C94" t="s">
         <v>96</v>
@@ -5079,7 +5184,7 @@
         <v>1</v>
       </c>
       <c r="I94" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J94" t="s">
         <v>118</v>
@@ -5098,23 +5203,23 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5152,7 +5257,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -5166,35 +5271,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B3" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C3" t="s">
         <v>92</v>
       </c>
       <c r="D3" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="F3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B4" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C4" t="s">
         <v>92</v>
       </c>
       <c r="D4" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E4" t="s">
         <v>53</v>
@@ -5203,12 +5308,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B5" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C5" t="s">
         <v>92</v>
@@ -5217,7 +5322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>52</v>
       </c>
@@ -5234,7 +5339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -5248,7 +5353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -5262,7 +5367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -5292,25 +5397,25 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A5" sqref="A5:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5348,7 +5453,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -5362,86 +5467,86 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B3" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C3" t="s">
         <v>92</v>
       </c>
       <c r="D3" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="F3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>342</v>
+      </c>
+      <c r="B4" t="s">
+        <v>346</v>
+      </c>
+      <c r="C4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" t="s">
+        <v>352</v>
+      </c>
+      <c r="F4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="F5" s="5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="F6" s="5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>344</v>
       </c>
-      <c r="B4" t="s">
-        <v>348</v>
-      </c>
-      <c r="C4" t="s">
-        <v>92</v>
-      </c>
-      <c r="D4" t="s">
-        <v>354</v>
-      </c>
-      <c r="F4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>345</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="B7" t="s">
         <v>349</v>
-      </c>
-      <c r="C5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D5" t="s">
-        <v>101</v>
-      </c>
-      <c r="E5" t="s">
-        <v>132</v>
-      </c>
-      <c r="F5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>337</v>
-      </c>
-      <c r="B6" t="s">
-        <v>350</v>
-      </c>
-      <c r="C6" t="s">
-        <v>92</v>
-      </c>
-      <c r="D6" t="s">
-        <v>101</v>
-      </c>
-      <c r="E6" t="s">
-        <v>132</v>
-      </c>
-      <c r="F6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>346</v>
-      </c>
-      <c r="B7" t="s">
-        <v>351</v>
       </c>
       <c r="C7" t="s">
         <v>96</v>
@@ -5450,12 +5555,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B8" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C8" t="s">
         <v>94</v>
@@ -5464,12 +5569,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B9" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C9" t="s">
         <v>94</v>
@@ -5478,7 +5583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>52</v>
       </c>
@@ -5495,7 +5600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>132</v>
       </c>
@@ -5509,13 +5614,13 @@
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="H11" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="J11" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
   </sheetData>
@@ -5528,26 +5633,26 @@
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="52.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5585,12 +5690,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B2" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C2" t="s">
         <v>92</v>
@@ -5602,7 +5707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -5616,12 +5721,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B4" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C4" t="s">
         <v>92</v>
@@ -5630,18 +5735,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B5" t="s">
+        <v>358</v>
+      </c>
+      <c r="C5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" t="s">
         <v>360</v>
-      </c>
-      <c r="C5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D5" t="s">
-        <v>362</v>
       </c>
       <c r="E5" t="s">
         <v>53</v>
@@ -5650,18 +5755,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B6" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C6" t="s">
         <v>94</v>
       </c>
       <c r="D6" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="E6" t="s">
         <v>53</v>
@@ -5670,10 +5775,10 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -5690,7 +5795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -5704,7 +5809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -5718,7 +5823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>53</v>
       </c>
@@ -5747,11 +5852,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5789,7 +5909,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -5803,12 +5923,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B3" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C3" t="s">
         <v>96</v>
@@ -5817,190 +5937,190 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B4" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C4" t="s">
         <v>97</v>
       </c>
       <c r="E4" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C5" t="s">
         <v>97</v>
       </c>
       <c r="E5" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="F5" t="b">
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B6" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C6" t="s">
         <v>97</v>
       </c>
       <c r="E6" t="s">
+        <v>373</v>
+      </c>
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>367</v>
+      </c>
+      <c r="B7" t="s">
         <v>375</v>
-      </c>
-      <c r="F6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I6" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>369</v>
-      </c>
-      <c r="B7" t="s">
-        <v>377</v>
       </c>
       <c r="C7" t="s">
         <v>97</v>
       </c>
       <c r="E7" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="F7" t="b">
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B8" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C8" t="s">
         <v>97</v>
       </c>
       <c r="E8" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="F8" t="b">
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B9" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C9" t="s">
         <v>97</v>
       </c>
       <c r="E9" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="F9" t="b">
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B10" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C10" t="s">
         <v>97</v>
       </c>
       <c r="E10" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="F10" t="b">
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B11" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C11" t="s">
         <v>97</v>
       </c>
       <c r="E11" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="F11" t="b">
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B12" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C12" t="s">
         <v>97</v>
       </c>
       <c r="E12" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="F12" t="b">
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>52</v>
       </c>
@@ -6028,9 +6148,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6068,7 +6188,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -6082,12 +6202,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B3" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C3" t="s">
         <v>96</v>
@@ -6096,90 +6216,90 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B4" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C4" t="s">
         <v>97</v>
       </c>
       <c r="E4" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B5" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C5" t="s">
         <v>97</v>
       </c>
       <c r="E5" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="F5" t="b">
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B6" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C6" t="s">
         <v>97</v>
       </c>
       <c r="E6" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="F6" t="b">
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B7" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C7" t="s">
         <v>97</v>
       </c>
       <c r="E7" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="F7" t="b">
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>52</v>
       </c>
@@ -6209,23 +6329,23 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6263,7 +6383,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -6277,12 +6397,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B3" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C3" t="s">
         <v>92</v>
@@ -6291,9 +6411,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B4" t="s">
         <v>132</v>
@@ -6305,15 +6425,15 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B5" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C5" t="s">
         <v>97</v>
@@ -6325,21 +6445,21 @@
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B6" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C6" t="s">
         <v>92</v>
       </c>
       <c r="D6" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E6" t="s">
         <v>132</v>
@@ -6348,12 +6468,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B7" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C7" t="s">
         <v>97</v>
@@ -6365,21 +6485,21 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B8" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C8" t="s">
         <v>92</v>
       </c>
       <c r="D8" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E8" t="s">
         <v>132</v>
@@ -6388,7 +6508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>52</v>
       </c>
@@ -6405,7 +6525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -6419,12 +6539,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B11" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C11" t="s">
         <v>92</v>

</xml_diff>

<commit_message>
~ updated ccfgs files
</commit_message>
<xml_diff>
--- a/examples/oucru/oucru-13dx/resources/outputs/templates/ccfgs_13dx_data_fixed.xlsx
+++ b/examples/oucru/oucru-13dx/resources/outputs/templates/ccfgs_13dx_data_fixed.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kelda\Desktop\repositories\github\datablend\main\examples\oucru\oucru-13dx\resources\outputs\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bernard\Desktop\repositories\datablend\examples\oucru\oucru-13dx\resources\outputs\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{797A471D-4D2D-4CBD-992B-57CE6C968CC9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44CC3FF6-C94B-4505-9078-D90FBCD66B91}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ENROL" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1087" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="453">
   <si>
     <t>from_name</t>
   </si>
@@ -1360,9 +1360,6 @@
     <t>or admission?? Compare</t>
   </si>
   <si>
-    <t>skin_Rash?</t>
-  </si>
-  <si>
     <t>Note</t>
   </si>
   <si>
@@ -1385,6 +1382,12 @@
   </si>
   <si>
     <t>event_discharge</t>
+  </si>
+  <si>
+    <t>skin_Rash? Skin_Perfusion?</t>
+  </si>
+  <si>
+    <t>mechanical intervention for bleeding</t>
   </si>
 </sst>
 </file>
@@ -1408,7 +1411,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1430,6 +1433,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1472,7 +1481,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1483,6 +1492,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1823,8 +1833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2624,7 +2634,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2890,23 +2900,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="15" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
         <v>416</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="6" t="s">
         <v>430</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="6" t="s">
         <v>438</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="6" t="s">
         <v>419</v>
       </c>
-      <c r="F15" t="b">
+      <c r="F15" s="6" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2956,8 +2966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:XFD23"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3018,7 +3028,7 @@
         <v>10</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -3292,7 +3302,7 @@
         <v>124</v>
       </c>
       <c r="B18" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C18" t="s">
         <v>95</v>
@@ -3321,7 +3331,7 @@
         <v>0</v>
       </c>
       <c r="N19" s="5" t="s">
-        <v>443</v>
+        <v>451</v>
       </c>
     </row>
     <row r="20" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -3338,7 +3348,7 @@
         <v>0</v>
       </c>
       <c r="N20" s="3" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -3543,15 +3553,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M94"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="E90" sqref="E90"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B83" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="L89" sqref="L89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="79.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.5703125" customWidth="1"/>
     <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
@@ -3562,7 +3575,7 @@
     <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3599,8 +3612,11 @@
       <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" s="2" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -3614,7 +3630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -3628,7 +3644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>152</v>
       </c>
@@ -3642,7 +3658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>153</v>
       </c>
@@ -3656,7 +3672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>154</v>
       </c>
@@ -3670,7 +3686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>155</v>
       </c>
@@ -3684,7 +3700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>156</v>
       </c>
@@ -3698,7 +3714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -3718,7 +3734,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -3732,7 +3748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -3752,7 +3768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>118</v>
       </c>
@@ -3769,7 +3785,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>157</v>
       </c>
@@ -3783,7 +3799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>158</v>
       </c>
@@ -3803,7 +3819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>159</v>
       </c>
@@ -3823,7 +3839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>160</v>
       </c>
@@ -4178,7 +4194,7 @@
         <v>0</v>
       </c>
       <c r="M35" s="5" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="36" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -4198,7 +4214,7 @@
         <v>0</v>
       </c>
       <c r="M36" s="5" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="37" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -4218,7 +4234,7 @@
         <v>0</v>
       </c>
       <c r="M37" s="5" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
@@ -4271,6 +4287,9 @@
       <c r="F40" t="b">
         <v>0</v>
       </c>
+      <c r="M40" s="5" t="s">
+        <v>452</v>
+      </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
@@ -4288,6 +4307,9 @@
       <c r="F41" t="b">
         <v>0</v>
       </c>
+      <c r="M41" t="s">
+        <v>452</v>
+      </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
@@ -4305,6 +4327,9 @@
       <c r="F42" t="b">
         <v>0</v>
       </c>
+      <c r="M42" t="s">
+        <v>452</v>
+      </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
@@ -4508,7 +4533,7 @@
         <v>0</v>
       </c>
       <c r="M53" s="5" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
@@ -5096,10 +5121,10 @@
         <v>1</v>
       </c>
       <c r="L89" s="5" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="M89" s="5" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.25">
@@ -5200,7 +5225,7 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5397,7 +5422,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5405,7 +5430,7 @@
     <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="57.7109375" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
@@ -6326,7 +6351,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
~ updated OUCRU configuration files
</commit_message>
<xml_diff>
--- a/examples/oucru/oucru-13dx/resources/outputs/templates/ccfgs_13dx_data_fixed.xlsx
+++ b/examples/oucru/oucru-13dx/resources/outputs/templates/ccfgs_13dx_data_fixed.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bernard\Desktop\repositories\datablend\examples\oucru\oucru-13dx\resources\outputs\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kelda\Desktop\repositories\github\datablend\main\examples\oucru\oucru-13dx\resources\outputs\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44CC3FF6-C94B-4505-9078-D90FBCD66B91}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B015240C-F437-4AD4-880F-8A25960911E4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1245" yWindow="2235" windowWidth="25425" windowHeight="11145" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ENROL" sheetId="1" r:id="rId1"/>
@@ -24,12 +24,23 @@
     <sheet name="SEROLOGY" sheetId="9" r:id="rId9"/>
     <sheet name="LAB_DIAGNOSIS" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1096" uniqueCount="452">
   <si>
     <t>from_name</t>
   </si>
@@ -1376,9 +1387,6 @@
   </si>
   <si>
     <t>?</t>
-  </si>
-  <si>
-    <t>date discharge when death? Or date discharge or date_death?</t>
   </si>
   <si>
     <t>event_discharge</t>
@@ -1481,7 +1489,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1493,6 +1501,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1833,8 +1842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="K43" sqref="K43"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2633,8 +2642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2966,14 +2975,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:XFD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
@@ -3331,7 +3340,7 @@
         <v>0</v>
       </c>
       <c r="N19" s="5" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="20" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -3506,10 +3515,10 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B30" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C30" t="s">
         <v>96</v>
@@ -3517,19 +3526,19 @@
       <c r="F30" t="b">
         <v>1</v>
       </c>
-      <c r="J30" t="s">
-        <v>113</v>
-      </c>
-      <c r="K30" t="s">
+      <c r="G30" t="s">
         <v>17</v>
+      </c>
+      <c r="H30" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C31" t="s">
         <v>96</v>
@@ -3537,11 +3546,11 @@
       <c r="F31" t="b">
         <v>1</v>
       </c>
-      <c r="G31" t="s">
-        <v>132</v>
-      </c>
-      <c r="H31" t="s">
-        <v>120</v>
+      <c r="J31" t="s">
+        <v>113</v>
+      </c>
+      <c r="K31" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -3551,13 +3560,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:M94"/>
+  <dimension ref="A1:M95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B83" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B62" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L89" sqref="L89"/>
+      <selection pane="bottomRight" activeCell="M90" sqref="M90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4288,7 +4297,7 @@
         <v>0</v>
       </c>
       <c r="M40" s="5" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
@@ -4308,7 +4317,7 @@
         <v>0</v>
       </c>
       <c r="M41" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
@@ -4328,7 +4337,7 @@
         <v>0</v>
       </c>
       <c r="M42" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
@@ -4971,7 +4980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>224</v>
       </c>
@@ -4988,7 +4997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>225</v>
       </c>
@@ -5008,7 +5017,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>226</v>
       </c>
@@ -5022,7 +5031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>227</v>
       </c>
@@ -5039,7 +5048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>228</v>
       </c>
@@ -5059,7 +5068,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>229</v>
       </c>
@@ -5073,7 +5082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>230</v>
       </c>
@@ -5093,7 +5102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>231</v>
       </c>
@@ -5107,7 +5116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
         <v>232</v>
       </c>
@@ -5121,13 +5130,10 @@
         <v>1</v>
       </c>
       <c r="L89" s="5" t="s">
-        <v>450</v>
-      </c>
-      <c r="M89" s="5" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>233</v>
       </c>
@@ -5144,7 +5150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>234</v>
       </c>
@@ -5158,7 +5164,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>52</v>
       </c>
@@ -5175,7 +5181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>235</v>
       </c>
@@ -5195,7 +5201,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>236</v>
       </c>
@@ -5213,6 +5219,29 @@
       </c>
       <c r="J94" t="s">
         <v>118</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>54</v>
+      </c>
+      <c r="B95" t="s">
+        <v>54</v>
+      </c>
+      <c r="C95" t="s">
+        <v>96</v>
+      </c>
+      <c r="F95" t="b">
+        <v>1</v>
+      </c>
+      <c r="I95" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="J95" t="s">
+        <v>118</v>
+      </c>
+      <c r="L95" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
~ ccfg files updated
</commit_message>
<xml_diff>
--- a/examples/oucru/oucru-13dx/resources/outputs/templates/ccfgs_13dx_data_fixed.xlsx
+++ b/examples/oucru/oucru-13dx/resources/outputs/templates/ccfgs_13dx_data_fixed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kelda\Desktop\repositories\github\datablend\main\examples\oucru\oucru-13dx\resources\outputs\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE966B4B-77F4-4979-A7BB-F5FA37D06286}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30993962-4998-427A-A0B3-4E0AC4D43FE6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25425" yWindow="480" windowWidth="23430" windowHeight="16470" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25530" yWindow="930" windowWidth="22290" windowHeight="16470" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ENROL" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1096" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1123" uniqueCount="457">
   <si>
     <t>from_name</t>
   </si>
@@ -462,9 +462,6 @@
     <t>which_ward</t>
   </si>
   <si>
-    <t>measure_pos</t>
-  </si>
-  <si>
     <t>time_temp</t>
   </si>
   <si>
@@ -495,9 +492,6 @@
     <t>{3: 'V_0', 1: 'V_1', 2: 'V_3', 9: 'V_4'}</t>
   </si>
   <si>
-    <t>{1: 'V_1', 2: 'V_2'}</t>
-  </si>
-  <si>
     <t>DateAssess</t>
   </si>
   <si>
@@ -765,9 +759,6 @@
     <t>birth_date_y</t>
   </si>
   <si>
-    <t>day_illness</t>
-  </si>
-  <si>
     <t>care_type</t>
   </si>
   <si>
@@ -843,12 +834,6 @@
     <t>crystalloid</t>
   </si>
   <si>
-    <t>nasal_packing</t>
-  </si>
-  <si>
-    <t>gum_packing</t>
-  </si>
-  <si>
     <t>compression</t>
   </si>
   <si>
@@ -1396,6 +1381,36 @@
   </si>
   <si>
     <t>{0: 'Inconclusive', 1: 'Primary', 2: 'Secondary'}</t>
+  </si>
+  <si>
+    <t>packing_nose</t>
+  </si>
+  <si>
+    <t>packing_gum</t>
+  </si>
+  <si>
+    <t>{1: 'Arm Pit', 2: 'Mouth'}</t>
+  </si>
+  <si>
+    <t>body_temperature_location</t>
+  </si>
+  <si>
+    <t>day_from_illness</t>
+  </si>
+  <si>
+    <t>-DayIllness</t>
+  </si>
+  <si>
+    <t>They are all blank</t>
+  </si>
+  <si>
+    <t>In PCR</t>
+  </si>
+  <si>
+    <t>In serology</t>
+  </si>
+  <si>
+    <t>In NS1</t>
   </si>
 </sst>
 </file>
@@ -1842,8 +1857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1904,7 +1919,7 @@
         <v>12</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -2123,6 +2138,9 @@
       <c r="C15" t="s">
         <v>94</v>
       </c>
+      <c r="E15" t="s">
+        <v>53</v>
+      </c>
       <c r="F15" t="b">
         <v>0</v>
       </c>
@@ -2137,6 +2155,9 @@
       <c r="C16" t="s">
         <v>94</v>
       </c>
+      <c r="E16" t="s">
+        <v>53</v>
+      </c>
       <c r="F16" t="b">
         <v>0</v>
       </c>
@@ -2484,6 +2505,9 @@
       <c r="D35" t="s">
         <v>100</v>
       </c>
+      <c r="E35" t="s">
+        <v>53</v>
+      </c>
       <c r="F35" t="b">
         <v>0</v>
       </c>
@@ -2498,6 +2522,9 @@
       <c r="C36" t="s">
         <v>93</v>
       </c>
+      <c r="E36" t="s">
+        <v>53</v>
+      </c>
       <c r="F36" t="b">
         <v>0</v>
       </c>
@@ -2512,6 +2539,9 @@
       <c r="C37" t="s">
         <v>94</v>
       </c>
+      <c r="E37" t="s">
+        <v>53</v>
+      </c>
       <c r="F37" t="b">
         <v>0</v>
       </c>
@@ -2630,7 +2660,7 @@
         <v>111</v>
       </c>
       <c r="N43" s="3" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
     </row>
   </sheetData>
@@ -2640,10 +2670,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2651,7 +2681,7 @@
     <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="117.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42" customWidth="1"/>
     <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
@@ -2662,7 +2692,7 @@
     <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2699,8 +2729,11 @@
       <c r="L1" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" s="2" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -2714,12 +2747,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="B3" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="C3" t="s">
         <v>94</v>
@@ -2728,12 +2761,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="B4" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="C4" t="s">
         <v>96</v>
@@ -2742,83 +2775,95 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>92</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="F5" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M5" s="3" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>92</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="F6" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M6" s="3" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>92</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="F7" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M7" s="3" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>92</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="F8" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M8" s="3" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>96</v>
@@ -2826,47 +2871,56 @@
       <c r="F9" s="3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M9" s="3" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>92</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="F10" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M10" s="3" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>92</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="F11" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M11" s="3" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>96</v>
@@ -2874,76 +2928,85 @@
       <c r="F12" s="3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M12" s="3" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>92</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="F13" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M13" s="3" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>92</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="F14" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M14" s="3" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>93</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="F15" s="6" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="B16" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="C16" t="s">
         <v>92</v>
       </c>
       <c r="D16" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="E16" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="F16" t="b">
         <v>0</v>
@@ -2975,8 +3038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:XFD30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3037,7 +3100,7 @@
         <v>10</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -3065,7 +3128,7 @@
         <v>92</v>
       </c>
       <c r="D3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F3" t="b">
         <v>0</v>
@@ -3096,7 +3159,7 @@
         <v>92</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F5" s="4" t="b">
         <v>0</v>
@@ -3113,7 +3176,7 @@
         <v>92</v>
       </c>
       <c r="D6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F6" t="b">
         <v>0</v>
@@ -3192,13 +3255,16 @@
         <v>119</v>
       </c>
       <c r="B11" t="s">
-        <v>140</v>
+        <v>450</v>
       </c>
       <c r="C11" t="s">
         <v>92</v>
       </c>
       <c r="D11" t="s">
-        <v>151</v>
+        <v>449</v>
+      </c>
+      <c r="E11" t="s">
+        <v>133</v>
       </c>
       <c r="F11" t="b">
         <v>0</v>
@@ -3209,7 +3275,7 @@
         <v>120</v>
       </c>
       <c r="B12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C12" t="s">
         <v>94</v>
@@ -3260,7 +3326,7 @@
         <v>121</v>
       </c>
       <c r="B15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C15" t="s">
         <v>95</v>
@@ -3277,7 +3343,7 @@
         <v>122</v>
       </c>
       <c r="B16" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C16" t="s">
         <v>95</v>
@@ -3294,7 +3360,7 @@
         <v>123</v>
       </c>
       <c r="B17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C17" t="s">
         <v>95</v>
@@ -3311,7 +3377,7 @@
         <v>124</v>
       </c>
       <c r="B18" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="C18" t="s">
         <v>95</v>
@@ -3328,7 +3394,7 @@
         <v>125</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>95</v>
@@ -3340,7 +3406,7 @@
         <v>0</v>
       </c>
       <c r="N19" s="5" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
     </row>
     <row r="20" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -3348,16 +3414,19 @@
         <v>126</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>95</v>
       </c>
+      <c r="E20" s="3" t="s">
+        <v>132</v>
+      </c>
       <c r="F20" s="3" t="b">
         <v>0</v>
       </c>
       <c r="N20" s="3" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -3365,7 +3434,7 @@
         <v>127</v>
       </c>
       <c r="B21" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C21" t="s">
         <v>95</v>
@@ -3563,10 +3632,10 @@
   <dimension ref="A1:M95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B62" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M90" sqref="M90"/>
+      <selection pane="bottomRight" activeCell="D96" sqref="D96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3578,7 +3647,7 @@
     <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" customWidth="1"/>
     <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
@@ -3622,7 +3691,7 @@
         <v>10</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -3655,10 +3724,10 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C4" t="s">
         <v>96</v>
@@ -3669,7 +3738,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B5" t="s">
         <v>61</v>
@@ -3683,10 +3752,10 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B6" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C6" t="s">
         <v>93</v>
@@ -3697,10 +3766,10 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B7" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C7" t="s">
         <v>93</v>
@@ -3711,10 +3780,10 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B8" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C8" t="s">
         <v>93</v>
@@ -3734,7 +3803,7 @@
         <v>93</v>
       </c>
       <c r="E9" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F9" t="b">
         <v>0</v>
@@ -3768,10 +3837,10 @@
         <v>92</v>
       </c>
       <c r="D11" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="E11" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F11" t="b">
         <v>0</v>
@@ -3796,33 +3865,36 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B13" t="s">
-        <v>241</v>
+        <v>451</v>
       </c>
       <c r="C13" t="s">
         <v>93</v>
       </c>
+      <c r="E13" t="s">
+        <v>235</v>
+      </c>
       <c r="F13" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B14" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C14" t="s">
         <v>92</v>
       </c>
       <c r="D14" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="E14" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F14" t="b">
         <v>0</v>
@@ -3830,10 +3902,10 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B15" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C15" t="s">
         <v>92</v>
@@ -3842,7 +3914,7 @@
         <v>100</v>
       </c>
       <c r="E15" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="F15" t="b">
         <v>0</v>
@@ -3850,10 +3922,10 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B16" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C16" t="s">
         <v>96</v>
@@ -3862,55 +3934,55 @@
         <v>1</v>
       </c>
       <c r="L16" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B17" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C17" t="s">
         <v>93</v>
       </c>
       <c r="E17" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F17" t="b">
         <v>0</v>
       </c>
       <c r="K17" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B18" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C18" t="s">
         <v>93</v>
       </c>
       <c r="E18" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F18" t="b">
         <v>0</v>
       </c>
       <c r="K18" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B19" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C19" t="s">
         <v>92</v>
@@ -3919,7 +3991,7 @@
         <v>100</v>
       </c>
       <c r="E19" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F19" t="b">
         <v>0</v>
@@ -3927,39 +3999,39 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B20" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C20" t="s">
         <v>93</v>
       </c>
       <c r="E20" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F20" t="b">
         <v>0</v>
       </c>
       <c r="K20" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B21" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C21" t="s">
         <v>92</v>
       </c>
       <c r="D21" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="E21" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F21" t="b">
         <v>0</v>
@@ -3967,10 +4039,10 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B22" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C22" t="s">
         <v>92</v>
@@ -3979,7 +4051,7 @@
         <v>100</v>
       </c>
       <c r="E22" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="F22" t="b">
         <v>0</v>
@@ -3987,19 +4059,19 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B23" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C23" t="s">
         <v>92</v>
       </c>
       <c r="D23" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="E23" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F23" t="b">
         <v>0</v>
@@ -4007,10 +4079,10 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B24" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C24" t="s">
         <v>96</v>
@@ -4021,7 +4093,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B25" t="s">
         <v>77</v>
@@ -4030,7 +4102,7 @@
         <v>95</v>
       </c>
       <c r="E25" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F25" t="b">
         <v>0</v>
@@ -4038,16 +4110,16 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B26" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C26" t="s">
         <v>95</v>
       </c>
       <c r="E26" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F26" t="b">
         <v>0</v>
@@ -4055,16 +4127,16 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B27" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C27" t="s">
         <v>95</v>
       </c>
       <c r="E27" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F27" t="b">
         <v>0</v>
@@ -4072,16 +4144,16 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B28" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C28" t="s">
         <v>95</v>
       </c>
       <c r="E28" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F28" t="b">
         <v>0</v>
@@ -4089,16 +4161,16 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B29" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C29" t="s">
         <v>95</v>
       </c>
       <c r="E29" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F29" t="b">
         <v>0</v>
@@ -4106,16 +4178,16 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B30" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C30" t="s">
         <v>95</v>
       </c>
       <c r="E30" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F30" t="b">
         <v>0</v>
@@ -4123,16 +4195,16 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B31" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C31" t="s">
         <v>95</v>
       </c>
       <c r="E31" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F31" t="b">
         <v>0</v>
@@ -4140,16 +4212,19 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B32" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C32" t="s">
         <v>92</v>
       </c>
       <c r="D32" t="s">
-        <v>322</v>
+        <v>317</v>
+      </c>
+      <c r="E32" t="s">
+        <v>249</v>
       </c>
       <c r="F32" t="b">
         <v>0</v>
@@ -4157,10 +4232,10 @@
     </row>
     <row r="33" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>92</v>
@@ -4168,96 +4243,102 @@
       <c r="D33" s="4" t="s">
         <v>100</v>
       </c>
+      <c r="E33" s="4" t="s">
+        <v>235</v>
+      </c>
       <c r="F33" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>95</v>
       </c>
+      <c r="E34" s="4" t="s">
+        <v>235</v>
+      </c>
       <c r="F34" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>95</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F35" s="5" t="b">
         <v>0</v>
       </c>
       <c r="M35" s="5" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
     </row>
     <row r="36" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>95</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F36" s="5" t="b">
         <v>0</v>
       </c>
       <c r="M36" s="5" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
     </row>
     <row r="37" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>95</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F37" s="5" t="b">
         <v>0</v>
       </c>
       <c r="M37" s="5" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B38" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C38" t="s">
         <v>95</v>
       </c>
       <c r="E38" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F38" t="b">
         <v>0</v>
@@ -4265,16 +4346,16 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B39" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C39" t="s">
         <v>95</v>
       </c>
       <c r="E39" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F39" t="b">
         <v>0</v>
@@ -4282,70 +4363,70 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B40" t="s">
-        <v>267</v>
+        <v>447</v>
       </c>
       <c r="C40" t="s">
         <v>95</v>
       </c>
       <c r="E40" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F40" t="b">
         <v>0</v>
       </c>
       <c r="M40" s="5" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B41" t="s">
-        <v>268</v>
+        <v>448</v>
       </c>
       <c r="C41" t="s">
         <v>95</v>
       </c>
       <c r="E41" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F41" t="b">
         <v>0</v>
       </c>
       <c r="M41" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B42" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="C42" t="s">
         <v>95</v>
       </c>
       <c r="E42" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F42" t="b">
         <v>0</v>
       </c>
       <c r="M42" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B43" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="C43" t="s">
         <v>94</v>
@@ -4356,10 +4437,10 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B44" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="C44" t="s">
         <v>92</v>
@@ -4368,7 +4449,7 @@
         <v>101</v>
       </c>
       <c r="E44" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="F44" t="b">
         <v>0</v>
@@ -4376,10 +4457,10 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B45" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="C45" t="s">
         <v>96</v>
@@ -4390,10 +4471,10 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B46" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="C46" t="s">
         <v>92</v>
@@ -4402,7 +4483,7 @@
         <v>100</v>
       </c>
       <c r="E46" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="F46" t="b">
         <v>0</v>
@@ -4410,10 +4491,10 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B47" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="C47" t="s">
         <v>92</v>
@@ -4422,7 +4503,7 @@
         <v>101</v>
       </c>
       <c r="E47" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="F47" t="b">
         <v>0</v>
@@ -4430,19 +4511,19 @@
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B48" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="C48" t="s">
         <v>92</v>
       </c>
       <c r="D48" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="E48" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="F48" t="b">
         <v>0</v>
@@ -4450,19 +4531,19 @@
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B49" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="C49" t="s">
         <v>92</v>
       </c>
       <c r="D49" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="E49" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="F49" t="b">
         <v>0</v>
@@ -4470,19 +4551,19 @@
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B50" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C50" t="s">
         <v>92</v>
       </c>
       <c r="D50" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="E50" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="F50" t="b">
         <v>0</v>
@@ -4490,10 +4571,10 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B51" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="C51" t="s">
         <v>95</v>
@@ -4504,10 +4585,10 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B52" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="C52" t="s">
         <v>92</v>
@@ -4516,7 +4597,7 @@
         <v>100</v>
       </c>
       <c r="E52" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F52" t="b">
         <v>0</v>
@@ -4524,10 +4605,10 @@
     </row>
     <row r="53" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>92</v>
@@ -4536,21 +4617,21 @@
         <v>101</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="F53" s="5" t="b">
         <v>0</v>
       </c>
       <c r="M53" s="5" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B54" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="C54" t="s">
         <v>96</v>
@@ -4561,10 +4642,10 @@
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B55" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="C55" t="s">
         <v>92</v>
@@ -4573,7 +4654,7 @@
         <v>100</v>
       </c>
       <c r="E55" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F55" t="b">
         <v>0</v>
@@ -4581,10 +4662,10 @@
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B56" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="C56" t="s">
         <v>92</v>
@@ -4593,7 +4674,7 @@
         <v>100</v>
       </c>
       <c r="E56" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F56" t="b">
         <v>0</v>
@@ -4601,10 +4682,10 @@
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B57" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="C57" t="s">
         <v>92</v>
@@ -4613,7 +4694,7 @@
         <v>101</v>
       </c>
       <c r="E57" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="F57" t="b">
         <v>0</v>
@@ -4621,10 +4702,10 @@
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B58" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="C58" t="s">
         <v>96</v>
@@ -4635,16 +4716,16 @@
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B59" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="C59" t="s">
         <v>95</v>
       </c>
       <c r="E59" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F59" t="b">
         <v>0</v>
@@ -4652,16 +4733,16 @@
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B60" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="C60" t="s">
         <v>95</v>
       </c>
       <c r="E60" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F60" t="b">
         <v>0</v>
@@ -4669,16 +4750,16 @@
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B61" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="C61" t="s">
         <v>95</v>
       </c>
       <c r="E61" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F61" t="b">
         <v>0</v>
@@ -4686,10 +4767,10 @@
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B62" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="C62" t="s">
         <v>95</v>
@@ -4700,16 +4781,16 @@
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B63" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="C63" t="s">
         <v>92</v>
       </c>
       <c r="D63" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="F63" t="b">
         <v>0</v>
@@ -4717,10 +4798,10 @@
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B64" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="C64" t="s">
         <v>92</v>
@@ -4729,7 +4810,7 @@
         <v>101</v>
       </c>
       <c r="E64" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="F64" t="b">
         <v>0</v>
@@ -4737,10 +4818,10 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B65" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="C65" t="s">
         <v>96</v>
@@ -4751,16 +4832,19 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B66" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="C66" t="s">
         <v>92</v>
       </c>
       <c r="D66" t="s">
-        <v>327</v>
+        <v>322</v>
+      </c>
+      <c r="E66" t="s">
+        <v>287</v>
       </c>
       <c r="F66" t="b">
         <v>0</v>
@@ -4768,10 +4852,10 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B67" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="C67" t="s">
         <v>92</v>
@@ -4780,7 +4864,7 @@
         <v>101</v>
       </c>
       <c r="E67" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="F67" t="b">
         <v>0</v>
@@ -4788,16 +4872,16 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B68" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="C68" t="s">
         <v>95</v>
       </c>
       <c r="E68" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F68" t="b">
         <v>0</v>
@@ -4814,7 +4898,7 @@
         <v>95</v>
       </c>
       <c r="E69" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F69" t="b">
         <v>0</v>
@@ -4822,16 +4906,16 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B70" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="C70" t="s">
         <v>95</v>
       </c>
       <c r="E70" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F70" t="b">
         <v>0</v>
@@ -4839,16 +4923,16 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B71" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="C71" t="s">
         <v>95</v>
       </c>
       <c r="E71" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F71" t="b">
         <v>0</v>
@@ -4856,10 +4940,10 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B72" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="C72" t="s">
         <v>95</v>
@@ -4870,10 +4954,10 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B73" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="C73" t="s">
         <v>94</v>
@@ -4884,10 +4968,10 @@
     </row>
     <row r="74" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="C74" s="4" t="s">
         <v>96</v>
@@ -4898,10 +4982,10 @@
     </row>
     <row r="75" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="C75" s="4" t="s">
         <v>93</v>
@@ -4912,10 +4996,10 @@
     </row>
     <row r="76" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="C76" s="4" t="s">
         <v>93</v>
@@ -4926,10 +5010,10 @@
     </row>
     <row r="77" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="C77" s="4" t="s">
         <v>93</v>
@@ -4940,10 +5024,10 @@
     </row>
     <row r="78" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="C78" s="4" t="s">
         <v>93</v>
@@ -4954,10 +5038,10 @@
     </row>
     <row r="79" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C79" s="4" t="s">
         <v>92</v>
@@ -4968,10 +5052,10 @@
     </row>
     <row r="80" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="C80" s="4" t="s">
         <v>93</v>
@@ -4982,16 +5066,16 @@
     </row>
     <row r="81" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="C81" s="4" t="s">
         <v>93</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F81" s="4" t="b">
         <v>0</v>
@@ -4999,30 +5083,30 @@
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B82" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="C82" t="s">
         <v>93</v>
       </c>
       <c r="E82" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F82" t="b">
         <v>0</v>
       </c>
       <c r="K82" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B83" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="C83" t="s">
         <v>93</v>
@@ -5033,16 +5117,16 @@
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B84" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="C84" t="s">
         <v>93</v>
       </c>
       <c r="E84" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F84" t="b">
         <v>0</v>
@@ -5050,30 +5134,30 @@
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B85" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="C85" t="s">
         <v>93</v>
       </c>
       <c r="E85" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F85" t="b">
         <v>0</v>
       </c>
       <c r="K85" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B86" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="C86" t="s">
         <v>93</v>
@@ -5084,19 +5168,19 @@
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B87" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="C87" t="s">
         <v>92</v>
       </c>
       <c r="D87" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="E87" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="F87" t="b">
         <v>0</v>
@@ -5104,24 +5188,27 @@
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B88" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="C88" t="s">
         <v>94</v>
       </c>
+      <c r="E88" t="s">
+        <v>310</v>
+      </c>
       <c r="F88" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="C89" s="5" t="s">
         <v>96</v>
@@ -5130,21 +5217,21 @@
         <v>1</v>
       </c>
       <c r="L89" s="5" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B90" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="C90" t="s">
         <v>94</v>
       </c>
       <c r="E90" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="F90" t="b">
         <v>0</v>
@@ -5152,10 +5239,10 @@
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B91" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="C91" t="s">
         <v>96</v>
@@ -5183,10 +5270,10 @@
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B93" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C93" t="s">
         <v>96</v>
@@ -5195,7 +5282,7 @@
         <v>1</v>
       </c>
       <c r="I93" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="J93" t="s">
         <v>118</v>
@@ -5203,10 +5290,10 @@
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B94" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C94" t="s">
         <v>96</v>
@@ -5215,7 +5302,7 @@
         <v>1</v>
       </c>
       <c r="I94" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="J94" t="s">
         <v>118</v>
@@ -5235,7 +5322,7 @@
         <v>1</v>
       </c>
       <c r="I95" s="7" t="s">
-        <v>157</v>
+        <v>452</v>
       </c>
       <c r="J95" t="s">
         <v>118</v>
@@ -5327,16 +5414,16 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="B3" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="C3" t="s">
         <v>92</v>
       </c>
       <c r="D3" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="F3" t="b">
         <v>0</v>
@@ -5344,16 +5431,16 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="B4" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="C4" t="s">
         <v>92</v>
       </c>
       <c r="D4" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="E4" t="s">
         <v>53</v>
@@ -5364,10 +5451,10 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="B5" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="C5" t="s">
         <v>92</v>
@@ -5523,16 +5610,16 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="B3" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="C3" t="s">
         <v>92</v>
       </c>
       <c r="D3" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="F3" t="b">
         <v>0</v>
@@ -5540,16 +5627,16 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="B4" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="C4" t="s">
         <v>92</v>
       </c>
       <c r="D4" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
@@ -5557,10 +5644,10 @@
     </row>
     <row r="5" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>92</v>
@@ -5577,10 +5664,10 @@
     </row>
     <row r="6" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>92</v>
@@ -5597,10 +5684,10 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>339</v>
+      </c>
+      <c r="B7" t="s">
         <v>344</v>
-      </c>
-      <c r="B7" t="s">
-        <v>349</v>
       </c>
       <c r="C7" t="s">
         <v>96</v>
@@ -5611,10 +5698,10 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>340</v>
+      </c>
+      <c r="B8" t="s">
         <v>345</v>
-      </c>
-      <c r="B8" t="s">
-        <v>350</v>
       </c>
       <c r="C8" t="s">
         <v>94</v>
@@ -5625,10 +5712,10 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="B9" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="C9" t="s">
         <v>94</v>
@@ -5668,13 +5755,13 @@
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="H11" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="J11" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
     </row>
   </sheetData>
@@ -5746,10 +5833,10 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="B2" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="C2" t="s">
         <v>92</v>
@@ -5777,10 +5864,10 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="B4" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="C4" t="s">
         <v>92</v>
@@ -5791,16 +5878,16 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>350</v>
+      </c>
+      <c r="B5" t="s">
+        <v>353</v>
+      </c>
+      <c r="C5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" t="s">
         <v>355</v>
-      </c>
-      <c r="B5" t="s">
-        <v>358</v>
-      </c>
-      <c r="C5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D5" t="s">
-        <v>360</v>
       </c>
       <c r="E5" t="s">
         <v>53</v>
@@ -5811,16 +5898,16 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="B6" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="C6" t="s">
         <v>94</v>
       </c>
       <c r="D6" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="E6" t="s">
         <v>53</v>
@@ -5829,7 +5916,7 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -5979,10 +6066,10 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="B3" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="C3" t="s">
         <v>96</v>
@@ -5991,187 +6078,187 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="B4" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="C4" t="s">
         <v>97</v>
       </c>
       <c r="E4" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="B5" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="C5" t="s">
         <v>97</v>
       </c>
       <c r="E5" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="F5" t="b">
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="B6" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="C6" t="s">
         <v>97</v>
       </c>
       <c r="E6" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="F6" t="b">
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="B7" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="C7" t="s">
         <v>97</v>
       </c>
       <c r="E7" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="F7" t="b">
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="B8" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="C8" t="s">
         <v>97</v>
       </c>
       <c r="E8" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="F8" t="b">
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="B9" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="C9" t="s">
         <v>97</v>
       </c>
       <c r="E9" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="F9" t="b">
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="B10" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="C10" t="s">
         <v>97</v>
       </c>
       <c r="E10" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="F10" t="b">
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="B11" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="C11" t="s">
         <v>97</v>
       </c>
       <c r="E11" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="F11" t="b">
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="B12" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="C12" t="s">
         <v>97</v>
       </c>
       <c r="E12" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="F12" t="b">
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -6203,6 +6290,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="20.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -6258,10 +6348,10 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="B3" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="C3" t="s">
         <v>96</v>
@@ -6270,87 +6360,87 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="B4" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="C4" t="s">
         <v>97</v>
       </c>
       <c r="E4" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="B5" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="C5" t="s">
         <v>97</v>
       </c>
       <c r="E5" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="F5" t="b">
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="B6" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="C6" t="s">
         <v>97</v>
       </c>
       <c r="E6" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="F6" t="b">
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="B7" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="C7" t="s">
         <v>97</v>
       </c>
       <c r="E7" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="F7" t="b">
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -6377,10 +6467,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6399,7 +6489,7 @@
     <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6436,8 +6526,11 @@
       <c r="L1" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" s="2" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -6451,12 +6544,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="B3" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="C3" t="s">
         <v>92</v>
@@ -6465,9 +6558,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="B4" t="s">
         <v>132</v>
@@ -6479,15 +6572,15 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>388</v>
+      </c>
+      <c r="B5" t="s">
         <v>393</v>
-      </c>
-      <c r="B5" t="s">
-        <v>398</v>
       </c>
       <c r="C5" t="s">
         <v>97</v>
@@ -6499,21 +6592,21 @@
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>389</v>
+      </c>
+      <c r="B6" t="s">
         <v>394</v>
       </c>
-      <c r="B6" t="s">
-        <v>399</v>
-      </c>
       <c r="C6" t="s">
         <v>92</v>
       </c>
       <c r="D6" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="E6" t="s">
         <v>132</v>
@@ -6522,12 +6615,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>390</v>
+      </c>
+      <c r="B7" t="s">
         <v>395</v>
-      </c>
-      <c r="B7" t="s">
-        <v>400</v>
       </c>
       <c r="C7" t="s">
         <v>97</v>
@@ -6539,21 +6632,21 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>391</v>
+      </c>
+      <c r="B8" t="s">
         <v>396</v>
       </c>
-      <c r="B8" t="s">
-        <v>401</v>
-      </c>
       <c r="C8" t="s">
         <v>92</v>
       </c>
       <c r="D8" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="E8" t="s">
         <v>132</v>
@@ -6562,7 +6655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>52</v>
       </c>
@@ -6579,32 +6672,38 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C10" t="s">
-        <v>92</v>
-      </c>
-      <c r="F10" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="C10" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F10" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>397</v>
       </c>
-      <c r="B11" t="s">
-        <v>402</v>
-      </c>
-      <c r="C11" t="s">
-        <v>92</v>
-      </c>
-      <c r="F11" t="b">
-        <v>0</v>
+      <c r="C11" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F11" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
   </sheetData>

</xml_diff>